<commit_message>
staff import improved also new columns added
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_staffs.xlsx
+++ b/public/uploads/media/default/sample_staffs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohamedjagne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BD2847-272F-40BA-BE77-5889E5A7CFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249F5C86-AB54-4863-84E1-6225F701D2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_staffs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>employee_id</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>base_salary</t>
+  </si>
+  <si>
+    <t>time_sheet_based</t>
+  </si>
+  <si>
+    <t>max_overtime_hours</t>
+  </si>
+  <si>
+    <t>working_hours</t>
   </si>
 </sst>
 </file>
@@ -437,32 +446,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,19 +513,28 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>129092</v>
       </c>
@@ -546,16 +568,25 @@
       <c r="K2" s="1">
         <v>44927</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2">
+        <v>8</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="S2">
         <v>63656563</v>
       </c>
     </row>

</xml_diff>